<commit_message>
F70 Xerife Edition com Alcance de 4000 km
</commit_message>
<xml_diff>
--- a/01_aircraft_survey.xlsx
+++ b/01_aircraft_survey.xlsx
@@ -1,13 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eloia\Desktop\PEE\2. Fase 2\Trabalho_Ney\aircraft-optimization\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7BB1C9-45AD-4D01-8F94-D86853892773}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Hints" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hints" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -242,7 +259,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -252,35 +269,37 @@
   </numFmts>
   <fonts count="6">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Inconsolata"/>
     </font>
@@ -290,7 +309,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -312,7 +331,13 @@
     </fill>
   </fills>
   <borders count="24">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF4C4C4C"/>
@@ -323,6 +348,8 @@
       <top style="medium">
         <color rgb="FF4C4C4C"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -331,6 +358,9 @@
       <right style="medium">
         <color rgb="FF4C4C4C"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -339,22 +369,31 @@
       <right style="medium">
         <color rgb="FF4C4C4C"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF4C4C4C"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FFF3F3F3"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -366,11 +405,17 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -379,14 +424,20 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -395,9 +446,11 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -412,32 +465,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="FFEFEFEF"/>
-      </right>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFEFEFEF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFEFEFEF"/>
-      </right>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -448,17 +476,36 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="medium">
         <color rgb="FFEFEFEF"/>
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FFEFEFEF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFEFEFEF"/>
+      </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -467,22 +514,58 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFEFEFEF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="medium">
         <color rgb="FFEFEFEF"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -491,211 +574,211 @@
       <right style="medium">
         <color rgb="FFEFEFEF"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="62">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="2" fontId="4" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="17" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="18" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="13" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="2" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="2" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="18" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="2" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="3" fontId="4" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="4" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="4" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="3" fontId="4" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="17" fillId="3" fontId="4" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="18" fillId="3" fontId="4" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="3" fontId="4" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="4" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="167" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="14" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="15" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="19" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="20" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="21" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="22" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="23" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -706,11 +789,17 @@
     <xdr:ext cx="4305300" cy="3209925"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png"/>
+        <xdr:cNvPr id="2" name="image2.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -734,11 +823,17 @@
     <xdr:ext cx="5505450" cy="4267200"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png"/>
+        <xdr:cNvPr id="3" name="image1.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -756,7 +851,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -946,55 +1041,55 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K1004"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="36.14"/>
-    <col customWidth="1" min="3" max="3" width="33.0"/>
-    <col customWidth="1" min="4" max="4" width="17.14"/>
-    <col customWidth="1" min="5" max="5" width="20.71"/>
-    <col customWidth="1" min="6" max="6" width="18.0"/>
-    <col customWidth="1" min="7" max="7" width="9.0"/>
-    <col customWidth="1" min="8" max="8" width="9.86"/>
-    <col customWidth="1" min="9" max="10" width="7.0"/>
-    <col customWidth="1" min="11" max="11" width="39.29"/>
-    <col customWidth="1" min="12" max="27" width="7.0"/>
+    <col min="1" max="2" width="36.140625" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="10" width="7" customWidth="1"/>
+    <col min="11" max="11" width="39.28515625" customWidth="1"/>
+    <col min="12" max="27" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6">
       <c r="A3" s="1"/>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6">
       <c r="A6" s="6"/>
       <c r="B6" s="7" t="s">
         <v>3</v>
@@ -1003,7 +1098,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6">
       <c r="A7" s="6"/>
       <c r="B7" s="9" t="s">
         <v>5</v>
@@ -1012,40 +1107,40 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6">
       <c r="B8" s="11"/>
       <c r="C8" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6">
       <c r="B9" s="11"/>
       <c r="C9" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6">
       <c r="A10" s="6"/>
       <c r="B10" s="11"/>
       <c r="C10" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6">
       <c r="A11" s="6"/>
       <c r="B11" s="11"/>
       <c r="C11" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6">
       <c r="A12" s="6"/>
       <c r="B12" s="12"/>
       <c r="C12" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6">
       <c r="A13" s="6"/>
       <c r="B13" s="14"/>
       <c r="C13" s="15"/>
@@ -1053,7 +1148,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="15"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6">
       <c r="A14" s="6"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -1061,7 +1156,7 @@
       <c r="E14" s="16"/>
       <c r="F14" s="15"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6">
       <c r="A15" s="6"/>
       <c r="B15" s="17" t="s">
         <v>12</v>
@@ -1079,83 +1174,83 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6">
       <c r="A16" s="6"/>
       <c r="B16" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="21">
-        <v>38600.0</v>
+        <v>38600</v>
       </c>
       <c r="D16" s="22">
-        <v>36740.0</v>
+        <v>36740</v>
       </c>
       <c r="E16" s="23">
-        <v>32999.0</v>
+        <v>32999</v>
       </c>
       <c r="F16" s="24">
-        <f t="shared" ref="F16:F31" si="1">AVERAGE(C16,D16,E16)</f>
+        <f t="shared" ref="F16:F31" si="0">AVERAGE(C16,D16,E16)</f>
         <v>36113</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6">
       <c r="A17" s="6"/>
       <c r="B17" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="26">
-        <v>20150.0</v>
+        <v>20150</v>
       </c>
       <c r="D17" s="27">
-        <v>22784.0</v>
+        <v>22784</v>
       </c>
       <c r="E17" s="28">
-        <v>19731.0</v>
+        <v>19731</v>
       </c>
       <c r="F17" s="24">
-        <f t="shared" si="1"/>
-        <v>20888.33333</v>
-      </c>
-    </row>
-    <row r="18">
+        <f t="shared" si="0"/>
+        <v>20888.333333333332</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="6"/>
       <c r="B18" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="21">
-        <v>9743.0</v>
+        <v>9743</v>
       </c>
       <c r="D18" s="22">
-        <v>10890.0</v>
+        <v>10890</v>
       </c>
       <c r="E18" s="23">
-        <v>8527.0</v>
+        <v>8527</v>
       </c>
       <c r="F18" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9720</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6">
       <c r="A19" s="6"/>
       <c r="B19" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="30">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="D19" s="27">
-        <v>79.0</v>
+        <v>79</v>
       </c>
       <c r="E19" s="28">
-        <v>78.0</v>
+        <v>78</v>
       </c>
       <c r="F19" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6">
       <c r="A20" s="6"/>
       <c r="B20" s="20" t="s">
         <v>21</v>
@@ -1170,30 +1265,30 @@
         <v>15.5</v>
       </c>
       <c r="F20" s="31">
-        <f t="shared" si="1"/>
-        <v>14.22333333</v>
-      </c>
-    </row>
-    <row r="21">
+        <f t="shared" si="0"/>
+        <v>14.223333333333334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="6"/>
       <c r="B21" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="26">
-        <v>3982.0</v>
+        <v>3982</v>
       </c>
       <c r="D21" s="27">
-        <v>2009.0</v>
+        <v>2009</v>
       </c>
       <c r="E21" s="28">
-        <v>2256.0</v>
+        <v>2256</v>
       </c>
       <c r="F21" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2749</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6">
       <c r="A22" s="6"/>
       <c r="B22" s="32" t="s">
         <v>23</v>
@@ -1208,11 +1303,11 @@
         <v>0.78</v>
       </c>
       <c r="F22" s="33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.79</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:6">
       <c r="A23" s="6"/>
       <c r="B23" s="25" t="s">
         <v>24</v>
@@ -1223,11 +1318,11 @@
       <c r="D23" s="34"/>
       <c r="E23" s="35"/>
       <c r="F23" s="36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10058.4</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6">
       <c r="A24" s="6"/>
       <c r="B24" s="20" t="s">
         <v>25</v>
@@ -1236,55 +1331,55 @@
         <v>12496.8</v>
       </c>
       <c r="D24" s="22">
-        <v>11000.0</v>
+        <v>11000</v>
       </c>
       <c r="E24" s="23">
-        <v>12497.0</v>
+        <v>12497</v>
       </c>
       <c r="F24" s="36">
-        <f t="shared" si="1"/>
-        <v>11997.93333</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>11997.933333333334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="A25" s="6"/>
       <c r="B25" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="26">
-        <v>1644.0</v>
+        <v>1644</v>
       </c>
       <c r="D25" s="27">
-        <v>1300.0</v>
+        <v>1300</v>
       </c>
       <c r="E25" s="28">
-        <v>1564.0</v>
+        <v>1564</v>
       </c>
       <c r="F25" s="24">
-        <f t="shared" si="1"/>
-        <v>1502.666667</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>1502.6666666666667</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26" s="6"/>
       <c r="B26" s="20" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="21">
-        <v>1241.0</v>
+        <v>1241</v>
       </c>
       <c r="D26" s="22">
-        <v>1210.0</v>
+        <v>1210</v>
       </c>
       <c r="E26" s="23">
-        <v>1540.0</v>
+        <v>1540</v>
       </c>
       <c r="F26" s="24">
-        <f t="shared" si="1"/>
-        <v>1330.333333</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>1330.3333333333333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1">
       <c r="A27" s="6"/>
       <c r="B27" s="25" t="s">
         <v>28</v>
@@ -1299,11 +1394,11 @@
         <v>70.61</v>
       </c>
       <c r="F27" s="33">
-        <f t="shared" si="1"/>
-        <v>78.94333333</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>78.943333333333328</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1">
       <c r="A28" s="6"/>
       <c r="B28" s="32" t="s">
         <v>29</v>
@@ -1318,11 +1413,11 @@
         <v>7.6</v>
       </c>
       <c r="F28" s="36">
-        <f t="shared" si="1"/>
-        <v>8.2</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>8.2000000000000011</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1">
       <c r="A29" s="6"/>
       <c r="B29" s="29" t="s">
         <v>30</v>
@@ -1331,36 +1426,36 @@
         <v>0.26</v>
       </c>
       <c r="D29" s="27">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E29" s="38">
-        <v>0.277</v>
+        <v>0.27700000000000002</v>
       </c>
       <c r="F29" s="31">
-        <f t="shared" si="1"/>
-        <v>0.2723333333</v>
-      </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>0.27233333333333337</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1">
       <c r="A30" s="6"/>
       <c r="B30" s="20" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="21">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="D30" s="22">
-        <v>19.9</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="E30" s="23">
         <v>23.44</v>
       </c>
       <c r="F30" s="31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21.78</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1">
       <c r="A31" s="6"/>
       <c r="B31" s="25" t="s">
         <v>32</v>
@@ -1369,17 +1464,17 @@
         <v>5.5</v>
       </c>
       <c r="D31" s="27">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E31" s="28">
         <v>1.86</v>
       </c>
       <c r="F31" s="33">
-        <f t="shared" si="1"/>
-        <v>3.453333333</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
+        <f t="shared" si="0"/>
+        <v>3.4533333333333331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1">
       <c r="A32" s="6"/>
       <c r="B32" s="32" t="s">
         <v>33</v>
@@ -1397,7 +1492,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:11" ht="15.75" customHeight="1">
       <c r="A33" s="6"/>
       <c r="B33" s="25" t="s">
         <v>35</v>
@@ -1412,12 +1507,12 @@
         <v>14.5</v>
       </c>
       <c r="F33" s="31">
-        <f t="shared" ref="F33:F45" si="2">AVERAGE(C33,D33,E33)</f>
-        <v>20.19666667</v>
+        <f t="shared" ref="F33:F45" si="1">AVERAGE(C33,D33,E33)</f>
+        <v>20.196666666666669</v>
       </c>
       <c r="K33" s="40"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:11" ht="15.75" customHeight="1">
       <c r="A34" s="6"/>
       <c r="B34" s="32" t="s">
         <v>36</v>
@@ -1432,11 +1527,11 @@
         <v>4.84</v>
       </c>
       <c r="F34" s="31">
-        <f t="shared" si="2"/>
-        <v>4.516666667</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
+        <f t="shared" si="1"/>
+        <v>4.5166666666666666</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1">
       <c r="A35" s="6"/>
       <c r="B35" s="29" t="s">
         <v>37</v>
@@ -1448,14 +1543,14 @@
         <v>0.42</v>
       </c>
       <c r="E35" s="28">
-        <v>0.446</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="F35" s="31">
-        <f t="shared" si="2"/>
-        <v>0.4453333333</v>
-      </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
+        <f t="shared" si="1"/>
+        <v>0.4453333333333333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" customHeight="1">
       <c r="A36" s="6"/>
       <c r="B36" s="20" t="s">
         <v>38</v>
@@ -1470,17 +1565,17 @@
         <v>28.5</v>
       </c>
       <c r="F36" s="31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>27.38</v>
       </c>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:11" ht="15.75" customHeight="1">
       <c r="A37" s="6"/>
       <c r="B37" s="25" t="s">
         <v>39</v>
       </c>
       <c r="C37" s="26">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="D37" s="27">
         <v>4.2</v>
@@ -1489,11 +1584,11 @@
         <v>-4.72</v>
       </c>
       <c r="F37" s="33">
-        <f t="shared" si="2"/>
-        <v>2.493333333</v>
-      </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
+        <f t="shared" si="1"/>
+        <v>2.4933333333333332</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" customHeight="1">
       <c r="A38" s="6"/>
       <c r="B38" s="32" t="s">
         <v>40</v>
@@ -1506,14 +1601,14 @@
       </c>
       <c r="E38" s="42">
         <f>16.22/3.4276</f>
-        <v>4.732174116</v>
+        <v>4.7321741159995332</v>
       </c>
       <c r="F38" s="31">
-        <f t="shared" si="2"/>
-        <v>4.027391372</v>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
+        <f t="shared" si="1"/>
+        <v>4.027391371999844</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1">
       <c r="A39" s="6"/>
       <c r="B39" s="29" t="s">
         <v>41</v>
@@ -1526,14 +1621,14 @@
       </c>
       <c r="E39" s="38">
         <f>E38*14.5/70.61</f>
-        <v>0.9717678046</v>
+        <v>0.97176780458848921</v>
       </c>
       <c r="F39" s="31">
-        <f t="shared" si="2"/>
-        <v>1.017255935</v>
-      </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
+        <f t="shared" si="1"/>
+        <v>1.0172559348628296</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1">
       <c r="A40" s="6"/>
       <c r="B40" s="20" t="s">
         <v>42</v>
@@ -1548,49 +1643,49 @@
         <v>9.67</v>
       </c>
       <c r="F40" s="31">
-        <f t="shared" si="2"/>
-        <v>13.42666667</v>
-      </c>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
+        <f t="shared" si="1"/>
+        <v>13.426666666666668</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" customHeight="1">
       <c r="A41" s="6"/>
       <c r="B41" s="29" t="s">
         <v>43</v>
       </c>
       <c r="C41" s="26">
-        <v>2.178</v>
+        <v>2.1779999999999999</v>
       </c>
       <c r="D41" s="27">
-        <v>1.184</v>
+        <v>1.1839999999999999</v>
       </c>
       <c r="E41" s="28">
         <v>1.06</v>
       </c>
       <c r="F41" s="31">
-        <f t="shared" si="2"/>
-        <v>1.474</v>
-      </c>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
+        <f t="shared" si="1"/>
+        <v>1.4740000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" customHeight="1">
       <c r="A42" s="6"/>
       <c r="B42" s="32" t="s">
         <v>44</v>
       </c>
       <c r="C42" s="21">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D42" s="22">
-        <v>0.704</v>
+        <v>0.70399999999999996</v>
       </c>
       <c r="E42" s="43">
-        <v>0.664</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="F42" s="31">
-        <f t="shared" si="2"/>
-        <v>0.5526666667</v>
-      </c>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
+        <f t="shared" si="1"/>
+        <v>0.55266666666666664</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1">
       <c r="A43" s="6"/>
       <c r="B43" s="25" t="s">
         <v>45</v>
@@ -1602,14 +1697,14 @@
         <v>38.57</v>
       </c>
       <c r="E43" s="28">
-        <v>38.13</v>
+        <v>38.130000000000003</v>
       </c>
       <c r="F43" s="33">
-        <f t="shared" si="2"/>
-        <v>37.48666667</v>
-      </c>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
+        <f t="shared" si="1"/>
+        <v>37.486666666666672</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1">
       <c r="A44" s="6"/>
       <c r="B44" s="20" t="s">
         <v>46</v>
@@ -1622,34 +1717,34 @@
       </c>
       <c r="E44" s="44">
         <f>13.53/24.85</f>
-        <v>0.5444668008</v>
+        <v>0.5444668008048289</v>
       </c>
       <c r="F44" s="33">
-        <f t="shared" si="2"/>
-        <v>0.4548222669</v>
-      </c>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
+        <f t="shared" si="1"/>
+        <v>0.45482226693494293</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" customHeight="1">
       <c r="A45" s="6"/>
       <c r="B45" s="29" t="s">
         <v>47</v>
       </c>
       <c r="C45" s="26">
-        <v>0.096</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="D45" s="27">
         <v>0.06</v>
       </c>
       <c r="E45" s="45">
         <f>E44*9.67/70.61</f>
-        <v>0.07456442379</v>
+        <v>7.4564423789586387E-2</v>
       </c>
       <c r="F45" s="31">
-        <f t="shared" si="2"/>
-        <v>0.07685480793</v>
-      </c>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
+        <f t="shared" si="1"/>
+        <v>7.6854807929862129E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" customHeight="1">
       <c r="A46" s="6"/>
       <c r="B46" s="32" t="s">
         <v>48</v>
@@ -1667,7 +1762,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" spans="1:11" ht="15.75" customHeight="1">
       <c r="A47" s="6"/>
       <c r="B47" s="25" t="s">
         <v>51</v>
@@ -1682,11 +1777,11 @@
         <v>33.5</v>
       </c>
       <c r="F47" s="36">
-        <f t="shared" ref="F47:F56" si="3">AVERAGE(C47,D47,E47)</f>
-        <v>31.43666667</v>
-      </c>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
+        <f t="shared" ref="F47:F56" si="2">AVERAGE(C47,D47,E47)</f>
+        <v>31.436666666666667</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" customHeight="1">
       <c r="A48" s="6"/>
       <c r="B48" s="20" t="s">
         <v>52</v>
@@ -1701,169 +1796,169 @@
         <v>2.74</v>
       </c>
       <c r="F48" s="33">
-        <f t="shared" si="3"/>
-        <v>3.13</v>
-      </c>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
+        <f t="shared" si="2"/>
+        <v>3.1300000000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" customHeight="1">
       <c r="A49" s="6"/>
       <c r="B49" s="29" t="s">
         <v>53</v>
       </c>
       <c r="C49" s="46">
         <f>3.72/3.35</f>
-        <v>1.110447761</v>
+        <v>1.1104477611940298</v>
       </c>
       <c r="D49" s="47">
         <f>3.81/3.3</f>
-        <v>1.154545455</v>
+        <v>1.1545454545454545</v>
       </c>
       <c r="E49" s="48">
         <f>3.27/E48</f>
-        <v>1.193430657</v>
+        <v>1.1934306569343065</v>
       </c>
       <c r="F49" s="31">
-        <f t="shared" si="3"/>
-        <v>1.152807958</v>
-      </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
+        <f t="shared" si="2"/>
+        <v>1.1528079575579302</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" customHeight="1">
       <c r="A50" s="6"/>
       <c r="B50" s="32" t="s">
         <v>54</v>
       </c>
       <c r="C50" s="49">
         <f>1.96/3.35</f>
-        <v>0.5850746269</v>
+        <v>0.58507462686567158</v>
       </c>
       <c r="D50" s="50">
         <f>1.76 /3.3</f>
-        <v>0.5333333333</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="E50" s="42">
         <f>2.25/E48</f>
-        <v>0.8211678832</v>
+        <v>0.82116788321167877</v>
       </c>
       <c r="F50" s="31">
-        <f t="shared" si="3"/>
-        <v>0.6465252811</v>
-      </c>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
+        <f t="shared" si="2"/>
+        <v>0.64652528113689456</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" customHeight="1">
       <c r="A51" s="6"/>
       <c r="B51" s="29" t="s">
         <v>55</v>
       </c>
       <c r="C51" s="26">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D51" s="27">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E51" s="28">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F51" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" spans="1:7" ht="15.75" customHeight="1">
       <c r="A52" s="6"/>
       <c r="B52" s="32" t="s">
         <v>56</v>
       </c>
       <c r="C52" s="21">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D52" s="22">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E52" s="23">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F52" s="24">
-        <f t="shared" si="3"/>
-        <v>1.666666667</v>
-      </c>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
+        <f t="shared" si="2"/>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" customHeight="1">
       <c r="A53" s="6"/>
       <c r="B53" s="25" t="s">
         <v>57</v>
       </c>
       <c r="C53" s="26">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D53" s="27">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E53" s="28">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F53" s="24">
-        <f t="shared" si="3"/>
-        <v>3.666666667</v>
-      </c>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
+        <f t="shared" si="2"/>
+        <v>3.6666666666666665</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" customHeight="1">
       <c r="A54" s="6"/>
       <c r="B54" s="32" t="s">
         <v>58</v>
       </c>
       <c r="C54" s="21">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="D54" s="22">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E54" s="23">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F54" s="24">
-        <f t="shared" si="3"/>
-        <v>4.666666667</v>
-      </c>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
+        <f t="shared" si="2"/>
+        <v>4.666666666666667</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" customHeight="1">
       <c r="A55" s="6"/>
       <c r="B55" s="29" t="s">
         <v>59</v>
       </c>
       <c r="C55" s="26">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D55" s="27">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E55" s="28">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F55" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" spans="1:7" ht="15.75" customHeight="1">
       <c r="A56" s="6"/>
       <c r="B56" s="32" t="s">
         <v>60</v>
       </c>
       <c r="C56" s="21">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D56" s="22">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E56" s="23">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F56" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
+    <row r="57" spans="1:7" ht="15.75" customHeight="1">
       <c r="A57" s="6"/>
       <c r="B57" s="29" t="s">
         <v>61</v>
@@ -1881,7 +1976,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
+    <row r="58" spans="1:7" ht="15.75" customHeight="1">
       <c r="A58" s="6"/>
       <c r="B58" s="20" t="s">
         <v>64</v>
@@ -1897,11 +1992,11 @@
         <v>112.8</v>
       </c>
       <c r="F58" s="33">
-        <f t="shared" ref="F58:F61" si="4">AVERAGE(C58,D58,E58)</f>
-        <v>121.6666667</v>
-      </c>
-    </row>
-    <row r="59" ht="15.75" customHeight="1">
+        <f t="shared" ref="F58:F61" si="3">AVERAGE(C58,D58,E58)</f>
+        <v>121.66666666666667</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" customHeight="1">
       <c r="A59" s="6"/>
       <c r="B59" s="25" t="s">
         <v>65</v>
@@ -1916,54 +2011,54 @@
         <v>0.67</v>
       </c>
       <c r="F59" s="33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.68</v>
       </c>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
+    <row r="60" spans="1:7" ht="15.75" customHeight="1">
       <c r="A60" s="6"/>
       <c r="B60" s="20" t="s">
         <v>66</v>
       </c>
       <c r="C60" s="49">
-        <v>530.80308</v>
+        <v>530.80308000000002</v>
       </c>
       <c r="D60" s="51">
-        <v>392.9411765</v>
+        <v>392.94117649999998</v>
       </c>
       <c r="E60" s="42">
-        <v>467.3417363</v>
+        <v>467.34173629999998</v>
       </c>
       <c r="F60" s="31">
-        <f t="shared" si="4"/>
-        <v>463.6953309</v>
+        <f t="shared" si="3"/>
+        <v>463.69533093333331</v>
       </c>
       <c r="G60" s="52"/>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
+    <row r="61" spans="1:7" ht="15.75" customHeight="1">
       <c r="A61" s="6"/>
       <c r="B61" s="29" t="s">
         <v>67</v>
       </c>
       <c r="C61" s="46">
         <f>C58/(C16*9.81*0.001)</f>
-        <v>0.3406696139</v>
+        <v>0.34066961385495398</v>
       </c>
       <c r="D61" s="47">
         <f>0.3418</f>
-        <v>0.3418</v>
+        <v>0.34179999999999999</v>
       </c>
       <c r="E61" s="48">
         <f>0.348804633</f>
-        <v>0.348804633</v>
+        <v>0.34880463299999998</v>
       </c>
       <c r="F61" s="31">
-        <f t="shared" si="4"/>
-        <v>0.3437580823</v>
+        <f t="shared" si="3"/>
+        <v>0.34375808228498467</v>
       </c>
       <c r="G61" s="52"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" spans="1:7" ht="15.75" customHeight="1">
       <c r="A62" s="6"/>
       <c r="B62" s="32" t="s">
         <v>68</v>
@@ -1981,82 +2076,82 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
+    <row r="63" spans="1:7" ht="15.75" customHeight="1">
       <c r="A63" s="6"/>
       <c r="B63" s="29" t="s">
         <v>70</v>
       </c>
       <c r="C63" s="26">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D63" s="27">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E63" s="28">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F63" s="54">
-        <f t="shared" ref="F63:F64" si="5">AVERAGE(C63,D63,E63)</f>
+        <f t="shared" ref="F63:F64" si="4">AVERAGE(C63,D63,E63)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
+    <row r="64" spans="1:7" ht="15.75" customHeight="1">
       <c r="A64" s="6"/>
       <c r="B64" s="55" t="s">
         <v>71</v>
       </c>
       <c r="C64" s="56">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D64" s="57">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E64" s="58">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F64" s="59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
+    <row r="65" spans="1:1" ht="15.75" customHeight="1">
       <c r="A65" s="6"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" spans="1:1" ht="15.75" customHeight="1">
       <c r="A66" s="6"/>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" spans="1:1" ht="15.75" customHeight="1">
       <c r="A67" s="6"/>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
+    <row r="68" spans="1:1" ht="15.75" customHeight="1">
       <c r="A68" s="6"/>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
+    <row r="69" spans="1:1" ht="15.75" customHeight="1">
       <c r="A69" s="6"/>
     </row>
-    <row r="70" ht="15.75" customHeight="1">
+    <row r="70" spans="1:1" ht="15.75" customHeight="1">
       <c r="A70" s="6"/>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
+    <row r="71" spans="1:1" ht="15.75" customHeight="1">
       <c r="A71" s="6"/>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
+    <row r="72" spans="1:1" ht="15.75" customHeight="1">
       <c r="A72" s="6"/>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
+    <row r="73" spans="1:1" ht="15.75" customHeight="1">
       <c r="A73" s="6"/>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
+    <row r="74" spans="1:1" ht="15.75" customHeight="1">
       <c r="A74" s="6"/>
     </row>
-    <row r="75" ht="15.75" customHeight="1">
+    <row r="75" spans="1:1" ht="15.75" customHeight="1">
       <c r="A75" s="6"/>
     </row>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="76" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="77" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="78" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="79" spans="1:1" ht="15.75" customHeight="1"/>
+    <row r="80" spans="1:1" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1"/>
@@ -2982,58 +3077,54 @@
     <row r="1003" ht="15.75" customHeight="1"/>
     <row r="1004" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="9.0"/>
-    <col customWidth="1" min="7" max="13" width="7.0"/>
-    <col customWidth="1" min="14" max="14" width="18.29"/>
-    <col customWidth="1" min="15" max="15" width="8.29"/>
-    <col customWidth="1" min="16" max="26" width="7.0"/>
+    <col min="1" max="6" width="9" customWidth="1"/>
+    <col min="7" max="13" width="7" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" customWidth="1"/>
+    <col min="16" max="26" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1">
       <c r="A1" s="60" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1">
       <c r="A2" s="60" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="21" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="22" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:15" ht="15.75" customHeight="1">
       <c r="A23" s="60" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="24" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:15" ht="15.75" customHeight="1">
       <c r="O27" s="61"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:15" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -4003,8 +4094,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>